<commit_message>
This analysis contains an updated grand analysis which uses one model with treatment as a predictor. IT also contains family data (longitude and lattitude, as well as other variables
</commit_message>
<xml_diff>
--- a/Data_Moities/Bolt_Field_Data_May132020.xlsx
+++ b/Data_Moities/Bolt_Field_Data_May132020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardhonor/Documents/R/masters_thesis/Synthesis/Data_Moities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EFB0C4-407D-8040-A8A5-788578C4EE17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F874D925-1FBF-F649-8CEA-EF29B3AD4B6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{A8DB64A3-4E12-BA4A-A58D-23C912D9DA77}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="104">
   <si>
     <t>jbc</t>
   </si>
@@ -339,6 +339,12 @@
   </si>
   <si>
     <t>i125</t>
+  </si>
+  <si>
+    <t>Maple_Died</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -690,15 +696,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B6C336-9D38-E34F-978B-469DDC35CEF1}">
-  <dimension ref="A1:I558"/>
+  <dimension ref="A1:J558"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D558" sqref="D558"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -726,8 +732,11 @@
       <c r="I1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>9</v>
       </c>
@@ -756,7 +765,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>9</v>
       </c>
@@ -785,7 +794,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>9</v>
       </c>
@@ -805,7 +814,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>9</v>
       </c>
@@ -825,7 +834,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>9</v>
       </c>
@@ -845,7 +854,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>9</v>
       </c>
@@ -865,7 +874,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>9</v>
       </c>
@@ -885,7 +894,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>9</v>
       </c>
@@ -914,7 +923,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>9</v>
       </c>
@@ -934,7 +943,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>9</v>
       </c>
@@ -954,7 +963,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>9</v>
       </c>
@@ -974,7 +983,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>8</v>
       </c>
@@ -994,7 +1003,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>8</v>
       </c>
@@ -1014,7 +1023,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>8</v>
       </c>
@@ -1034,7 +1043,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1063,7 +1072,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>8</v>
       </c>
@@ -1092,7 +1101,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>8</v>
       </c>
@@ -1121,7 +1130,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>8</v>
       </c>
@@ -1150,7 +1159,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>8</v>
       </c>
@@ -1179,7 +1188,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>8</v>
       </c>
@@ -1199,7 +1208,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>8</v>
       </c>
@@ -1219,7 +1228,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>8</v>
       </c>
@@ -1239,7 +1248,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>8</v>
       </c>
@@ -1259,7 +1268,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>9</v>
       </c>
@@ -1278,8 +1287,11 @@
       <c r="I25" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>9</v>
       </c>
@@ -1299,7 +1311,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>9</v>
       </c>
@@ -1319,7 +1331,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>9</v>
       </c>
@@ -1339,7 +1351,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>9</v>
       </c>
@@ -1359,7 +1371,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>9</v>
       </c>
@@ -1379,7 +1391,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>9</v>
       </c>
@@ -1399,7 +1411,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>9</v>
       </c>
@@ -1727,7 +1739,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>9</v>
       </c>
@@ -1744,7 +1756,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>9</v>
       </c>
@@ -1761,7 +1773,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>9</v>
       </c>
@@ -1778,7 +1790,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>9</v>
       </c>
@@ -1807,7 +1819,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>9</v>
       </c>
@@ -1836,7 +1848,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>9</v>
       </c>
@@ -1865,7 +1877,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:10">
       <c r="A55">
         <v>9</v>
       </c>
@@ -1894,7 +1906,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:10">
       <c r="A56">
         <v>9</v>
       </c>
@@ -1911,7 +1923,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:10">
       <c r="A57">
         <v>9</v>
       </c>
@@ -1928,7 +1940,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:10">
       <c r="A58">
         <v>9</v>
       </c>
@@ -1945,7 +1957,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:10">
       <c r="A59">
         <v>9</v>
       </c>
@@ -1962,7 +1974,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:10">
       <c r="A60">
         <v>9</v>
       </c>
@@ -1990,8 +2002,11 @@
       <c r="I60" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="J60" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61">
         <v>9</v>
       </c>
@@ -2020,7 +2035,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:10">
       <c r="A62">
         <v>9</v>
       </c>
@@ -2036,8 +2051,11 @@
       <c r="I62" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="J62" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63">
         <v>9</v>
       </c>
@@ -2054,7 +2072,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:10">
       <c r="A64">
         <v>9</v>
       </c>
@@ -4407,7 +4425,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="177" spans="1:9">
+    <row r="177" spans="1:10">
       <c r="A177">
         <v>6</v>
       </c>
@@ -4436,7 +4454,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="178" spans="1:9">
+    <row r="178" spans="1:10">
       <c r="A178">
         <v>6</v>
       </c>
@@ -4453,7 +4471,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="179" spans="1:9">
+    <row r="179" spans="1:10">
       <c r="A179">
         <v>6</v>
       </c>
@@ -4470,7 +4488,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="180" spans="1:9">
+    <row r="180" spans="1:10">
       <c r="A180">
         <v>6</v>
       </c>
@@ -4487,7 +4505,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="181" spans="1:9">
+    <row r="181" spans="1:10">
       <c r="A181">
         <v>6</v>
       </c>
@@ -4504,7 +4522,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="182" spans="1:9">
+    <row r="182" spans="1:10">
       <c r="A182">
         <v>6</v>
       </c>
@@ -4533,7 +4551,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="183" spans="1:9">
+    <row r="183" spans="1:10">
       <c r="A183">
         <v>6</v>
       </c>
@@ -4550,7 +4568,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="184" spans="1:9">
+    <row r="184" spans="1:10">
       <c r="A184">
         <v>6</v>
       </c>
@@ -4567,7 +4585,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="185" spans="1:9">
+    <row r="185" spans="1:10">
       <c r="A185">
         <v>6</v>
       </c>
@@ -4583,8 +4601,11 @@
       <c r="I185" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="186" spans="1:9">
+      <c r="J185" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10">
       <c r="A186">
         <v>6</v>
       </c>
@@ -4601,7 +4622,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="187" spans="1:9">
+    <row r="187" spans="1:10">
       <c r="A187">
         <v>6</v>
       </c>
@@ -4630,7 +4651,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="188" spans="1:9">
+    <row r="188" spans="1:10">
       <c r="A188">
         <v>6</v>
       </c>
@@ -4647,7 +4668,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="189" spans="1:9">
+    <row r="189" spans="1:10">
       <c r="A189">
         <v>6</v>
       </c>
@@ -4676,7 +4697,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="190" spans="1:9">
+    <row r="190" spans="1:10">
       <c r="A190">
         <v>6</v>
       </c>
@@ -4693,7 +4714,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="191" spans="1:9">
+    <row r="191" spans="1:10">
       <c r="A191">
         <v>6</v>
       </c>
@@ -4710,7 +4731,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="192" spans="1:9">
+    <row r="192" spans="1:10">
       <c r="A192">
         <v>6</v>
       </c>
@@ -7125,6 +7146,9 @@
       <c r="D310">
         <v>541</v>
       </c>
+      <c r="I310" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="311" spans="1:9">
       <c r="A311">
@@ -7151,6 +7175,9 @@
       <c r="H311">
         <v>14</v>
       </c>
+      <c r="I311" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="312" spans="1:9">
       <c r="A312">
@@ -7177,6 +7204,9 @@
       <c r="H312">
         <v>7</v>
       </c>
+      <c r="I312" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="313" spans="1:9">
       <c r="A313">
@@ -7203,6 +7233,9 @@
       <c r="H313">
         <v>5</v>
       </c>
+      <c r="I313" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="314" spans="1:9">
       <c r="A314">
@@ -7229,6 +7262,9 @@
       <c r="H314">
         <v>4</v>
       </c>
+      <c r="I314" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="315" spans="1:9">
       <c r="A315">
@@ -7255,6 +7291,9 @@
       <c r="H315">
         <v>9</v>
       </c>
+      <c r="I315" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="316" spans="1:9">
       <c r="A316">
@@ -7281,6 +7320,9 @@
       <c r="H316">
         <v>8</v>
       </c>
+      <c r="I316" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="317" spans="1:9">
       <c r="A317">
@@ -7307,6 +7349,9 @@
       <c r="H317">
         <v>27</v>
       </c>
+      <c r="I317" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="318" spans="1:9">
       <c r="A318">
@@ -7333,6 +7378,9 @@
       <c r="H318">
         <v>2</v>
       </c>
+      <c r="I318" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="319" spans="1:9">
       <c r="A319">
@@ -7347,6 +7395,9 @@
       <c r="D319">
         <v>459</v>
       </c>
+      <c r="I319" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="320" spans="1:9">
       <c r="A320">
@@ -7361,8 +7412,11 @@
       <c r="D320">
         <v>290</v>
       </c>
-    </row>
-    <row r="321" spans="1:8">
+      <c r="I320" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="321" spans="1:10">
       <c r="A321">
         <v>2</v>
       </c>
@@ -7387,8 +7441,11 @@
       <c r="H321">
         <v>16</v>
       </c>
-    </row>
-    <row r="322" spans="1:8">
+      <c r="I321" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="322" spans="1:10">
       <c r="A322">
         <v>2</v>
       </c>
@@ -7401,8 +7458,11 @@
       <c r="D322" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="323" spans="1:8">
+      <c r="I322" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="323" spans="1:10">
       <c r="A323">
         <v>2</v>
       </c>
@@ -7415,8 +7475,11 @@
       <c r="D323">
         <v>306</v>
       </c>
-    </row>
-    <row r="324" spans="1:8">
+      <c r="I323" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="324" spans="1:10">
       <c r="A324">
         <v>2</v>
       </c>
@@ -7429,8 +7492,11 @@
       <c r="D324" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="325" spans="1:8">
+      <c r="I324" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="325" spans="1:10">
       <c r="A325">
         <v>2</v>
       </c>
@@ -7455,8 +7521,14 @@
       <c r="H325">
         <v>8</v>
       </c>
-    </row>
-    <row r="326" spans="1:8">
+      <c r="I325" t="s">
+        <v>59</v>
+      </c>
+      <c r="J325" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="326" spans="1:10">
       <c r="A326">
         <v>2</v>
       </c>
@@ -7469,8 +7541,11 @@
       <c r="D326">
         <v>15</v>
       </c>
-    </row>
-    <row r="327" spans="1:8">
+      <c r="I326" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="327" spans="1:10">
       <c r="A327">
         <v>2</v>
       </c>
@@ -7483,8 +7558,11 @@
       <c r="D327">
         <v>37</v>
       </c>
-    </row>
-    <row r="328" spans="1:8">
+      <c r="I327" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="328" spans="1:10">
       <c r="A328">
         <v>2</v>
       </c>
@@ -7497,8 +7575,11 @@
       <c r="D328">
         <v>5</v>
       </c>
-    </row>
-    <row r="329" spans="1:8">
+      <c r="I328" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="329" spans="1:10">
       <c r="A329">
         <v>2</v>
       </c>
@@ -7511,8 +7592,11 @@
       <c r="D329">
         <v>14</v>
       </c>
-    </row>
-    <row r="330" spans="1:8">
+      <c r="I329" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="330" spans="1:10">
       <c r="A330">
         <v>2</v>
       </c>
@@ -7525,8 +7609,11 @@
       <c r="D330">
         <v>176</v>
       </c>
-    </row>
-    <row r="331" spans="1:8">
+      <c r="I330" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="331" spans="1:10">
       <c r="A331">
         <v>2</v>
       </c>
@@ -7539,8 +7626,11 @@
       <c r="D331">
         <v>418</v>
       </c>
-    </row>
-    <row r="332" spans="1:8">
+      <c r="I331" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="332" spans="1:10">
       <c r="A332">
         <v>2</v>
       </c>
@@ -7565,8 +7655,11 @@
       <c r="H332">
         <v>17</v>
       </c>
-    </row>
-    <row r="333" spans="1:8">
+      <c r="I332" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="333" spans="1:10">
       <c r="A333">
         <v>2</v>
       </c>
@@ -7579,8 +7672,11 @@
       <c r="D333">
         <v>464</v>
       </c>
-    </row>
-    <row r="334" spans="1:8">
+      <c r="I333" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="334" spans="1:10">
       <c r="A334">
         <v>2</v>
       </c>
@@ -7593,8 +7689,11 @@
       <c r="D334">
         <v>246</v>
       </c>
-    </row>
-    <row r="335" spans="1:8">
+      <c r="I334" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="335" spans="1:10">
       <c r="A335">
         <v>2</v>
       </c>
@@ -7607,8 +7706,11 @@
       <c r="D335">
         <v>527</v>
       </c>
-    </row>
-    <row r="336" spans="1:8">
+      <c r="I335" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="336" spans="1:10">
       <c r="A336">
         <v>2</v>
       </c>
@@ -7621,8 +7723,11 @@
       <c r="D336">
         <v>58</v>
       </c>
-    </row>
-    <row r="337" spans="1:8">
+      <c r="I336" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="337" spans="1:9">
       <c r="A337">
         <v>2</v>
       </c>
@@ -7635,8 +7740,11 @@
       <c r="D337">
         <v>446</v>
       </c>
-    </row>
-    <row r="338" spans="1:8">
+      <c r="I337" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="338" spans="1:9">
       <c r="A338">
         <v>2</v>
       </c>
@@ -7649,8 +7757,11 @@
       <c r="D338">
         <v>324</v>
       </c>
-    </row>
-    <row r="339" spans="1:8">
+      <c r="I338" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="339" spans="1:9">
       <c r="A339">
         <v>2</v>
       </c>
@@ -7663,8 +7774,11 @@
       <c r="D339">
         <v>55</v>
       </c>
-    </row>
-    <row r="340" spans="1:8">
+      <c r="I339" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="340" spans="1:9">
       <c r="A340">
         <v>2</v>
       </c>
@@ -7677,8 +7791,11 @@
       <c r="D340">
         <v>272</v>
       </c>
-    </row>
-    <row r="341" spans="1:8">
+      <c r="I340" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="341" spans="1:9">
       <c r="A341">
         <v>2</v>
       </c>
@@ -7703,8 +7820,11 @@
       <c r="H341">
         <v>4</v>
       </c>
-    </row>
-    <row r="342" spans="1:8">
+      <c r="I341" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="342" spans="1:9">
       <c r="A342">
         <v>2</v>
       </c>
@@ -7717,8 +7837,11 @@
       <c r="D342" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="343" spans="1:8">
+      <c r="I342" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="343" spans="1:9">
       <c r="A343">
         <v>2</v>
       </c>
@@ -7731,8 +7854,11 @@
       <c r="D343">
         <v>409</v>
       </c>
-    </row>
-    <row r="344" spans="1:8">
+      <c r="I343" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="344" spans="1:9">
       <c r="A344">
         <v>2</v>
       </c>
@@ -7745,8 +7871,11 @@
       <c r="D344">
         <v>23</v>
       </c>
-    </row>
-    <row r="345" spans="1:8">
+      <c r="I344" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="345" spans="1:9">
       <c r="A345">
         <v>2</v>
       </c>
@@ -7759,8 +7888,11 @@
       <c r="D345">
         <v>314</v>
       </c>
-    </row>
-    <row r="346" spans="1:8">
+      <c r="I345" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="346" spans="1:9">
       <c r="A346">
         <v>2</v>
       </c>
@@ -7773,8 +7905,11 @@
       <c r="D346">
         <v>289</v>
       </c>
-    </row>
-    <row r="347" spans="1:8">
+      <c r="I346" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="347" spans="1:9">
       <c r="A347">
         <v>2</v>
       </c>
@@ -7787,8 +7922,11 @@
       <c r="D347">
         <v>120</v>
       </c>
-    </row>
-    <row r="348" spans="1:8">
+      <c r="I347" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="348" spans="1:9">
       <c r="A348">
         <v>2</v>
       </c>
@@ -7801,8 +7939,11 @@
       <c r="D348">
         <v>319</v>
       </c>
-    </row>
-    <row r="349" spans="1:8">
+      <c r="I348" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="349" spans="1:9">
       <c r="A349">
         <v>2</v>
       </c>
@@ -7815,8 +7956,11 @@
       <c r="D349">
         <v>392</v>
       </c>
-    </row>
-    <row r="350" spans="1:8">
+      <c r="I349" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="350" spans="1:9">
       <c r="A350">
         <v>2</v>
       </c>
@@ -7829,8 +7973,11 @@
       <c r="D350">
         <v>12</v>
       </c>
-    </row>
-    <row r="351" spans="1:8">
+      <c r="I350" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="351" spans="1:9">
       <c r="A351">
         <v>2</v>
       </c>
@@ -7843,8 +7990,11 @@
       <c r="D351">
         <v>560</v>
       </c>
-    </row>
-    <row r="352" spans="1:8">
+      <c r="I351" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="352" spans="1:9">
       <c r="A352">
         <v>2</v>
       </c>
@@ -7857,8 +8007,11 @@
       <c r="D352">
         <v>483</v>
       </c>
-    </row>
-    <row r="353" spans="1:8">
+      <c r="I352" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="353" spans="1:9">
       <c r="A353">
         <v>2</v>
       </c>
@@ -7871,8 +8024,11 @@
       <c r="D353">
         <v>251</v>
       </c>
-    </row>
-    <row r="354" spans="1:8">
+      <c r="I353" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="354" spans="1:9">
       <c r="A354">
         <v>2</v>
       </c>
@@ -7885,8 +8041,11 @@
       <c r="D354">
         <v>182</v>
       </c>
-    </row>
-    <row r="355" spans="1:8">
+      <c r="I354" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="355" spans="1:9">
       <c r="A355">
         <v>2</v>
       </c>
@@ -7899,8 +8058,11 @@
       <c r="D355">
         <v>92</v>
       </c>
-    </row>
-    <row r="356" spans="1:8">
+      <c r="I355" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="356" spans="1:9">
       <c r="A356">
         <v>2</v>
       </c>
@@ -7925,8 +8087,11 @@
       <c r="H356">
         <v>13</v>
       </c>
-    </row>
-    <row r="357" spans="1:8">
+      <c r="I356" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="357" spans="1:9">
       <c r="A357">
         <v>2</v>
       </c>
@@ -7951,8 +8116,11 @@
       <c r="H357">
         <v>9</v>
       </c>
-    </row>
-    <row r="358" spans="1:8">
+      <c r="I357" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="358" spans="1:9">
       <c r="A358">
         <v>2</v>
       </c>
@@ -7977,8 +8145,11 @@
       <c r="H358">
         <v>14</v>
       </c>
-    </row>
-    <row r="359" spans="1:8">
+      <c r="I358" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="359" spans="1:9">
       <c r="A359">
         <v>2</v>
       </c>
@@ -8003,8 +8174,11 @@
       <c r="H359">
         <v>7</v>
       </c>
-    </row>
-    <row r="360" spans="1:8">
+      <c r="I359" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="360" spans="1:9">
       <c r="A360">
         <v>2</v>
       </c>
@@ -8029,8 +8203,11 @@
       <c r="H360">
         <v>6</v>
       </c>
-    </row>
-    <row r="361" spans="1:8">
+      <c r="I360" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="361" spans="1:9">
       <c r="A361">
         <v>3</v>
       </c>
@@ -8043,8 +8220,11 @@
       <c r="D361">
         <v>187</v>
       </c>
-    </row>
-    <row r="362" spans="1:8">
+      <c r="I361" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="362" spans="1:9">
       <c r="A362">
         <v>3</v>
       </c>
@@ -8057,8 +8237,11 @@
       <c r="D362">
         <v>542</v>
       </c>
-    </row>
-    <row r="363" spans="1:8">
+      <c r="I362" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="363" spans="1:9">
       <c r="A363">
         <v>3</v>
       </c>
@@ -8083,8 +8266,11 @@
       <c r="H363">
         <v>38</v>
       </c>
-    </row>
-    <row r="364" spans="1:8">
+      <c r="I363" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="364" spans="1:9">
       <c r="A364">
         <v>3</v>
       </c>
@@ -8097,8 +8283,11 @@
       <c r="D364">
         <v>540</v>
       </c>
-    </row>
-    <row r="365" spans="1:8">
+      <c r="I364" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="365" spans="1:9">
       <c r="A365">
         <v>3</v>
       </c>
@@ -8123,8 +8312,11 @@
       <c r="H365">
         <v>9</v>
       </c>
-    </row>
-    <row r="366" spans="1:8">
+      <c r="I365" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="366" spans="1:9">
       <c r="A366">
         <v>3</v>
       </c>
@@ -8149,8 +8341,11 @@
       <c r="H366">
         <v>5</v>
       </c>
-    </row>
-    <row r="367" spans="1:8">
+      <c r="I366" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="367" spans="1:9">
       <c r="A367">
         <v>3</v>
       </c>
@@ -8175,8 +8370,11 @@
       <c r="H367">
         <v>11</v>
       </c>
-    </row>
-    <row r="368" spans="1:8">
+      <c r="I367" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="368" spans="1:9">
       <c r="A368">
         <v>3</v>
       </c>
@@ -8189,8 +8387,11 @@
       <c r="D368">
         <v>338</v>
       </c>
-    </row>
-    <row r="369" spans="1:8">
+      <c r="I368" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="369" spans="1:9">
       <c r="A369">
         <v>3</v>
       </c>
@@ -8215,8 +8416,11 @@
       <c r="H369">
         <v>12</v>
       </c>
-    </row>
-    <row r="370" spans="1:8">
+      <c r="I369" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="370" spans="1:9">
       <c r="A370">
         <v>3</v>
       </c>
@@ -8229,8 +8433,11 @@
       <c r="D370">
         <v>169</v>
       </c>
-    </row>
-    <row r="371" spans="1:8">
+      <c r="I370" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="371" spans="1:9">
       <c r="A371">
         <v>3</v>
       </c>
@@ -8255,8 +8462,11 @@
       <c r="H371">
         <v>2</v>
       </c>
-    </row>
-    <row r="372" spans="1:8">
+      <c r="I371" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="372" spans="1:9">
       <c r="A372">
         <v>3</v>
       </c>
@@ -8269,8 +8479,11 @@
       <c r="D372">
         <v>110</v>
       </c>
-    </row>
-    <row r="373" spans="1:8">
+      <c r="I372" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="373" spans="1:9">
       <c r="A373">
         <v>3</v>
       </c>
@@ -8295,8 +8508,11 @@
       <c r="H373">
         <v>6</v>
       </c>
-    </row>
-    <row r="374" spans="1:8">
+      <c r="I373" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="374" spans="1:9">
       <c r="A374">
         <v>3</v>
       </c>
@@ -8309,8 +8525,11 @@
       <c r="D374">
         <v>454</v>
       </c>
-    </row>
-    <row r="375" spans="1:8">
+      <c r="I374" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="375" spans="1:9">
       <c r="A375">
         <v>3</v>
       </c>
@@ -8323,8 +8542,11 @@
       <c r="D375">
         <v>333</v>
       </c>
-    </row>
-    <row r="376" spans="1:8">
+      <c r="I375" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="376" spans="1:9">
       <c r="A376">
         <v>3</v>
       </c>
@@ -8337,8 +8559,11 @@
       <c r="D376">
         <v>310</v>
       </c>
-    </row>
-    <row r="377" spans="1:8">
+      <c r="I376" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="377" spans="1:9">
       <c r="A377">
         <v>3</v>
       </c>
@@ -8351,8 +8576,11 @@
       <c r="D377">
         <v>505</v>
       </c>
-    </row>
-    <row r="378" spans="1:8">
+      <c r="I377" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="378" spans="1:9">
       <c r="A378">
         <v>3</v>
       </c>
@@ -8365,8 +8593,11 @@
       <c r="D378">
         <v>408</v>
       </c>
-    </row>
-    <row r="379" spans="1:8">
+      <c r="I378" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="379" spans="1:9">
       <c r="A379">
         <v>3</v>
       </c>
@@ -8379,8 +8610,11 @@
       <c r="D379">
         <v>288</v>
       </c>
-    </row>
-    <row r="380" spans="1:8">
+      <c r="I379" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="380" spans="1:9">
       <c r="A380">
         <v>3</v>
       </c>
@@ -8393,8 +8627,11 @@
       <c r="D380">
         <v>304</v>
       </c>
-    </row>
-    <row r="381" spans="1:8">
+      <c r="I380" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="381" spans="1:9">
       <c r="A381">
         <v>3</v>
       </c>
@@ -8407,8 +8644,11 @@
       <c r="D381">
         <v>531</v>
       </c>
-    </row>
-    <row r="382" spans="1:8">
+      <c r="I381" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="382" spans="1:9">
       <c r="A382">
         <v>3</v>
       </c>
@@ -8421,8 +8661,11 @@
       <c r="D382">
         <v>153</v>
       </c>
-    </row>
-    <row r="383" spans="1:8">
+      <c r="I382" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="383" spans="1:9">
       <c r="A383">
         <v>3</v>
       </c>
@@ -8447,8 +8690,11 @@
       <c r="H383">
         <v>10</v>
       </c>
-    </row>
-    <row r="384" spans="1:8">
+      <c r="I383" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="384" spans="1:9">
       <c r="A384">
         <v>3</v>
       </c>
@@ -8473,8 +8719,11 @@
       <c r="H384">
         <v>7</v>
       </c>
-    </row>
-    <row r="385" spans="1:8">
+      <c r="I384" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="385" spans="1:9">
       <c r="A385">
         <v>3</v>
       </c>
@@ -8499,8 +8748,11 @@
       <c r="H385">
         <v>22</v>
       </c>
-    </row>
-    <row r="386" spans="1:8">
+      <c r="I385" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="386" spans="1:9">
       <c r="A386">
         <v>3</v>
       </c>
@@ -8513,8 +8765,11 @@
       <c r="D386">
         <v>181</v>
       </c>
-    </row>
-    <row r="387" spans="1:8">
+      <c r="I386" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="387" spans="1:9">
       <c r="A387">
         <v>3</v>
       </c>
@@ -8527,8 +8782,11 @@
       <c r="D387">
         <v>570</v>
       </c>
-    </row>
-    <row r="388" spans="1:8">
+      <c r="I387" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="388" spans="1:9">
       <c r="A388">
         <v>3</v>
       </c>
@@ -8541,8 +8799,11 @@
       <c r="D388">
         <v>460</v>
       </c>
-    </row>
-    <row r="389" spans="1:8">
+      <c r="I388" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="389" spans="1:9">
       <c r="A389">
         <v>3</v>
       </c>
@@ -8567,8 +8828,11 @@
       <c r="H389">
         <v>1</v>
       </c>
-    </row>
-    <row r="390" spans="1:8">
+      <c r="I389" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="390" spans="1:9">
       <c r="A390">
         <v>3</v>
       </c>
@@ -8593,8 +8857,11 @@
       <c r="H390">
         <v>6</v>
       </c>
-    </row>
-    <row r="391" spans="1:8">
+      <c r="I390" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="391" spans="1:9">
       <c r="A391">
         <v>3</v>
       </c>
@@ -8607,8 +8874,11 @@
       <c r="D391">
         <v>536</v>
       </c>
-    </row>
-    <row r="392" spans="1:8">
+      <c r="I391" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="392" spans="1:9">
       <c r="A392">
         <v>3</v>
       </c>
@@ -8621,8 +8891,11 @@
       <c r="D392">
         <v>240</v>
       </c>
-    </row>
-    <row r="393" spans="1:8">
+      <c r="I392" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="393" spans="1:9">
       <c r="A393">
         <v>3</v>
       </c>
@@ -8635,8 +8908,11 @@
       <c r="D393">
         <v>185</v>
       </c>
-    </row>
-    <row r="394" spans="1:8">
+      <c r="I393" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="394" spans="1:9">
       <c r="A394">
         <v>3</v>
       </c>
@@ -8649,8 +8925,11 @@
       <c r="D394">
         <v>219</v>
       </c>
-    </row>
-    <row r="395" spans="1:8">
+      <c r="I394" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="395" spans="1:9">
       <c r="A395">
         <v>3</v>
       </c>
@@ -8663,8 +8942,11 @@
       <c r="D395">
         <v>470</v>
       </c>
-    </row>
-    <row r="396" spans="1:8">
+      <c r="I395" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="396" spans="1:9">
       <c r="A396">
         <v>3</v>
       </c>
@@ -8677,8 +8959,11 @@
       <c r="D396">
         <v>167</v>
       </c>
-    </row>
-    <row r="397" spans="1:8">
+      <c r="I396" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="397" spans="1:9">
       <c r="A397">
         <v>3</v>
       </c>
@@ -8703,8 +8988,11 @@
       <c r="H397">
         <v>4</v>
       </c>
-    </row>
-    <row r="398" spans="1:8">
+      <c r="I397" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="398" spans="1:9">
       <c r="A398">
         <v>3</v>
       </c>
@@ -8717,8 +9005,11 @@
       <c r="D398">
         <v>121</v>
       </c>
-    </row>
-    <row r="399" spans="1:8">
+      <c r="I398" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="399" spans="1:9">
       <c r="A399">
         <v>3</v>
       </c>
@@ -8731,8 +9022,11 @@
       <c r="D399">
         <v>566</v>
       </c>
-    </row>
-    <row r="400" spans="1:8">
+      <c r="I399" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="400" spans="1:9">
       <c r="A400">
         <v>3</v>
       </c>
@@ -8745,8 +9039,11 @@
       <c r="D400">
         <v>184</v>
       </c>
-    </row>
-    <row r="401" spans="1:8">
+      <c r="I400" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="401" spans="1:9">
       <c r="A401">
         <v>3</v>
       </c>
@@ -8759,8 +9056,11 @@
       <c r="D401">
         <v>17</v>
       </c>
-    </row>
-    <row r="402" spans="1:8">
+      <c r="I401" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="402" spans="1:9">
       <c r="A402">
         <v>3</v>
       </c>
@@ -8773,8 +9073,11 @@
       <c r="D402">
         <v>204</v>
       </c>
-    </row>
-    <row r="403" spans="1:8">
+      <c r="I402" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="403" spans="1:9">
       <c r="A403">
         <v>3</v>
       </c>
@@ -8787,8 +9090,11 @@
       <c r="D403">
         <v>525</v>
       </c>
-    </row>
-    <row r="404" spans="1:8">
+      <c r="I403" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="404" spans="1:9">
       <c r="A404">
         <v>3</v>
       </c>
@@ -8801,8 +9107,11 @@
       <c r="D404">
         <v>71</v>
       </c>
-    </row>
-    <row r="405" spans="1:8">
+      <c r="I404" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="405" spans="1:9">
       <c r="A405">
         <v>3</v>
       </c>
@@ -8827,8 +9136,11 @@
       <c r="H405">
         <v>3</v>
       </c>
-    </row>
-    <row r="406" spans="1:8">
+      <c r="I405" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="406" spans="1:9">
       <c r="A406">
         <v>3</v>
       </c>
@@ -8841,8 +9153,11 @@
       <c r="D406">
         <v>205</v>
       </c>
-    </row>
-    <row r="407" spans="1:8">
+      <c r="I406" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="407" spans="1:9">
       <c r="A407">
         <v>3</v>
       </c>
@@ -8855,8 +9170,11 @@
       <c r="D407">
         <v>368</v>
       </c>
-    </row>
-    <row r="408" spans="1:8">
+      <c r="I407" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="408" spans="1:9">
       <c r="A408">
         <v>3</v>
       </c>
@@ -8869,8 +9187,11 @@
       <c r="D408">
         <v>109</v>
       </c>
-    </row>
-    <row r="409" spans="1:8">
+      <c r="I408" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="409" spans="1:9">
       <c r="A409">
         <v>3</v>
       </c>
@@ -8883,8 +9204,11 @@
       <c r="D409">
         <v>503</v>
       </c>
-    </row>
-    <row r="410" spans="1:8">
+      <c r="I409" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="410" spans="1:9">
       <c r="A410">
         <v>3</v>
       </c>
@@ -8897,8 +9221,11 @@
       <c r="D410">
         <v>341</v>
       </c>
-    </row>
-    <row r="411" spans="1:8">
+      <c r="I410" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="411" spans="1:9">
       <c r="A411">
         <v>3</v>
       </c>
@@ -8923,8 +9250,11 @@
       <c r="H411">
         <v>10</v>
       </c>
-    </row>
-    <row r="412" spans="1:8">
+      <c r="I411" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="412" spans="1:9">
       <c r="A412">
         <v>3</v>
       </c>
@@ -8937,8 +9267,11 @@
       <c r="D412">
         <v>435</v>
       </c>
-    </row>
-    <row r="413" spans="1:8">
+      <c r="I412" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="413" spans="1:9">
       <c r="A413">
         <v>3</v>
       </c>
@@ -8951,8 +9284,11 @@
       <c r="D413" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="414" spans="1:8">
+      <c r="I413" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="414" spans="1:9">
       <c r="A414">
         <v>3</v>
       </c>
@@ -8965,8 +9301,11 @@
       <c r="D414">
         <v>165</v>
       </c>
-    </row>
-    <row r="415" spans="1:8">
+      <c r="I414" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="415" spans="1:9">
       <c r="A415">
         <v>3</v>
       </c>
@@ -8979,8 +9318,11 @@
       <c r="D415">
         <v>159</v>
       </c>
-    </row>
-    <row r="416" spans="1:8">
+      <c r="I415" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="416" spans="1:9">
       <c r="A416">
         <v>3</v>
       </c>
@@ -8993,8 +9335,11 @@
       <c r="D416">
         <v>462</v>
       </c>
-    </row>
-    <row r="417" spans="1:8">
+      <c r="I416" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="417" spans="1:9">
       <c r="A417">
         <v>3</v>
       </c>
@@ -9007,8 +9352,11 @@
       <c r="D417" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="418" spans="1:8">
+      <c r="I417" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="418" spans="1:9">
       <c r="A418">
         <v>3</v>
       </c>
@@ -9033,8 +9381,11 @@
       <c r="H418">
         <v>36</v>
       </c>
-    </row>
-    <row r="419" spans="1:8">
+      <c r="I418" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="419" spans="1:9">
       <c r="A419">
         <v>3</v>
       </c>
@@ -9047,8 +9398,11 @@
       <c r="D419">
         <v>186</v>
       </c>
-    </row>
-    <row r="420" spans="1:8">
+      <c r="I419" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="420" spans="1:9">
       <c r="A420">
         <v>3</v>
       </c>
@@ -9061,8 +9415,11 @@
       <c r="D420" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="421" spans="1:8">
+      <c r="I420" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="421" spans="1:9">
       <c r="A421">
         <v>3</v>
       </c>
@@ -9075,8 +9432,11 @@
       <c r="D421">
         <v>420</v>
       </c>
-    </row>
-    <row r="422" spans="1:8">
+      <c r="I421" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="422" spans="1:9">
       <c r="A422">
         <v>3</v>
       </c>
@@ -9101,8 +9461,11 @@
       <c r="H422">
         <v>9</v>
       </c>
-    </row>
-    <row r="423" spans="1:8">
+      <c r="I422" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="423" spans="1:9">
       <c r="A423">
         <v>3</v>
       </c>
@@ -9127,8 +9490,11 @@
       <c r="H423">
         <v>4</v>
       </c>
-    </row>
-    <row r="424" spans="1:8">
+      <c r="I423" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="424" spans="1:9">
       <c r="A424">
         <v>3</v>
       </c>
@@ -9141,8 +9507,11 @@
       <c r="D424">
         <v>428</v>
       </c>
-    </row>
-    <row r="425" spans="1:8">
+      <c r="I424" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="425" spans="1:9">
       <c r="A425">
         <v>3</v>
       </c>
@@ -9167,8 +9536,11 @@
       <c r="H425">
         <v>30</v>
       </c>
-    </row>
-    <row r="426" spans="1:8">
+      <c r="I425" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="426" spans="1:9">
       <c r="A426">
         <v>3</v>
       </c>
@@ -9181,8 +9553,11 @@
       <c r="D426">
         <v>128</v>
       </c>
-    </row>
-    <row r="427" spans="1:8">
+      <c r="I426" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="427" spans="1:9">
       <c r="A427">
         <v>3</v>
       </c>
@@ -9195,8 +9570,11 @@
       <c r="D427">
         <v>8</v>
       </c>
-    </row>
-    <row r="428" spans="1:8">
+      <c r="I427" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="428" spans="1:9">
       <c r="A428">
         <v>4</v>
       </c>
@@ -9209,8 +9587,11 @@
       <c r="D428">
         <v>320</v>
       </c>
-    </row>
-    <row r="429" spans="1:8">
+      <c r="I428" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="429" spans="1:9">
       <c r="A429">
         <v>4</v>
       </c>
@@ -9223,8 +9604,11 @@
       <c r="D429">
         <v>247</v>
       </c>
-    </row>
-    <row r="430" spans="1:8">
+      <c r="I429" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="430" spans="1:9">
       <c r="A430">
         <v>4</v>
       </c>
@@ -9249,8 +9633,11 @@
       <c r="H430">
         <v>14</v>
       </c>
-    </row>
-    <row r="431" spans="1:8">
+      <c r="I430" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="431" spans="1:9">
       <c r="A431">
         <v>4</v>
       </c>
@@ -9263,8 +9650,11 @@
       <c r="D431">
         <v>209</v>
       </c>
-    </row>
-    <row r="432" spans="1:8">
+      <c r="I431" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="432" spans="1:9">
       <c r="A432">
         <v>4</v>
       </c>
@@ -9289,8 +9679,11 @@
       <c r="H432">
         <v>9</v>
       </c>
-    </row>
-    <row r="433" spans="1:8">
+      <c r="I432" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="433" spans="1:9">
       <c r="A433">
         <v>4</v>
       </c>
@@ -9303,8 +9696,11 @@
       <c r="D433">
         <v>572</v>
       </c>
-    </row>
-    <row r="434" spans="1:8">
+      <c r="I433" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="434" spans="1:9">
       <c r="A434">
         <v>4</v>
       </c>
@@ -9329,8 +9725,11 @@
       <c r="H434">
         <v>13</v>
       </c>
-    </row>
-    <row r="435" spans="1:8">
+      <c r="I434" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="435" spans="1:9">
       <c r="A435">
         <v>4</v>
       </c>
@@ -9355,8 +9754,11 @@
       <c r="H435">
         <v>14</v>
       </c>
-    </row>
-    <row r="436" spans="1:8">
+      <c r="I435" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="436" spans="1:9">
       <c r="A436">
         <v>4</v>
       </c>
@@ -9381,8 +9783,11 @@
       <c r="H436">
         <v>11</v>
       </c>
-    </row>
-    <row r="437" spans="1:8">
+      <c r="I436" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="437" spans="1:9">
       <c r="A437">
         <v>4</v>
       </c>
@@ -9395,8 +9800,11 @@
       <c r="D437">
         <v>564</v>
       </c>
-    </row>
-    <row r="438" spans="1:8">
+      <c r="I437" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="438" spans="1:9">
       <c r="A438">
         <v>4</v>
       </c>
@@ -9421,8 +9829,11 @@
       <c r="H438">
         <v>7</v>
       </c>
-    </row>
-    <row r="439" spans="1:8">
+      <c r="I438" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="439" spans="1:9">
       <c r="A439">
         <v>4</v>
       </c>
@@ -9435,8 +9846,11 @@
       <c r="D439" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="440" spans="1:8">
+      <c r="I439" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="440" spans="1:9">
       <c r="A440">
         <v>4</v>
       </c>
@@ -9449,8 +9863,11 @@
       <c r="D440">
         <v>218</v>
       </c>
-    </row>
-    <row r="441" spans="1:8">
+      <c r="I440" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="441" spans="1:9">
       <c r="A441">
         <v>4</v>
       </c>
@@ -9475,8 +9892,11 @@
       <c r="H441">
         <v>10</v>
       </c>
-    </row>
-    <row r="442" spans="1:8">
+      <c r="I441" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="442" spans="1:9">
       <c r="A442">
         <v>4</v>
       </c>
@@ -9501,8 +9921,11 @@
       <c r="H442">
         <v>17</v>
       </c>
-    </row>
-    <row r="443" spans="1:8">
+      <c r="I442" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="443" spans="1:9">
       <c r="A443">
         <v>4</v>
       </c>
@@ -9527,8 +9950,11 @@
       <c r="H443">
         <v>20</v>
       </c>
-    </row>
-    <row r="444" spans="1:8">
+      <c r="I443" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="444" spans="1:9">
       <c r="A444">
         <v>4</v>
       </c>
@@ -9553,8 +9979,11 @@
       <c r="H444">
         <v>10</v>
       </c>
-    </row>
-    <row r="445" spans="1:8">
+      <c r="I444" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="445" spans="1:9">
       <c r="A445">
         <v>4</v>
       </c>
@@ -9579,8 +10008,11 @@
       <c r="H445">
         <v>15</v>
       </c>
-    </row>
-    <row r="446" spans="1:8">
+      <c r="I445" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="446" spans="1:9">
       <c r="A446">
         <v>4</v>
       </c>
@@ -9605,8 +10037,11 @@
       <c r="H446">
         <v>15</v>
       </c>
-    </row>
-    <row r="447" spans="1:8">
+      <c r="I446" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="447" spans="1:9">
       <c r="A447">
         <v>4</v>
       </c>
@@ -9631,8 +10066,11 @@
       <c r="H447">
         <v>9</v>
       </c>
-    </row>
-    <row r="448" spans="1:8">
+      <c r="I447" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="448" spans="1:9">
       <c r="A448">
         <v>4</v>
       </c>
@@ -9657,8 +10095,11 @@
       <c r="H448">
         <v>16</v>
       </c>
-    </row>
-    <row r="449" spans="1:8">
+      <c r="I448" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="449" spans="1:9">
       <c r="A449">
         <v>4</v>
       </c>
@@ -9671,8 +10112,11 @@
       <c r="D449">
         <v>80</v>
       </c>
-    </row>
-    <row r="450" spans="1:8">
+      <c r="I449" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="450" spans="1:9">
       <c r="A450">
         <v>4</v>
       </c>
@@ -9685,8 +10129,11 @@
       <c r="D450">
         <v>287</v>
       </c>
-    </row>
-    <row r="451" spans="1:8">
+      <c r="I450" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="451" spans="1:9">
       <c r="A451">
         <v>4</v>
       </c>
@@ -9711,8 +10158,11 @@
       <c r="H451">
         <v>32</v>
       </c>
-    </row>
-    <row r="452" spans="1:8">
+      <c r="I451" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="452" spans="1:9">
       <c r="A452">
         <v>4</v>
       </c>
@@ -9725,8 +10175,11 @@
       <c r="D452">
         <v>39</v>
       </c>
-    </row>
-    <row r="453" spans="1:8">
+      <c r="I452" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="453" spans="1:9">
       <c r="A453">
         <v>4</v>
       </c>
@@ -9739,8 +10192,11 @@
       <c r="D453">
         <v>158</v>
       </c>
-    </row>
-    <row r="454" spans="1:8">
+      <c r="I453" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="454" spans="1:9">
       <c r="A454">
         <v>4</v>
       </c>
@@ -9753,8 +10209,11 @@
       <c r="D454">
         <v>50</v>
       </c>
-    </row>
-    <row r="455" spans="1:8">
+      <c r="I454" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="455" spans="1:9">
       <c r="A455">
         <v>4</v>
       </c>
@@ -9767,8 +10226,11 @@
       <c r="D455">
         <v>111</v>
       </c>
-    </row>
-    <row r="456" spans="1:8">
+      <c r="I455" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="456" spans="1:9">
       <c r="A456">
         <v>4</v>
       </c>
@@ -9781,8 +10243,11 @@
       <c r="D456">
         <v>510</v>
       </c>
-    </row>
-    <row r="457" spans="1:8">
+      <c r="I456" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="457" spans="1:9">
       <c r="A457">
         <v>4</v>
       </c>
@@ -9807,8 +10272,11 @@
       <c r="H457">
         <v>20</v>
       </c>
-    </row>
-    <row r="458" spans="1:8">
+      <c r="I457" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="458" spans="1:9">
       <c r="A458">
         <v>4</v>
       </c>
@@ -9833,8 +10301,11 @@
       <c r="H458">
         <v>6</v>
       </c>
-    </row>
-    <row r="459" spans="1:8">
+      <c r="I458" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="459" spans="1:9">
       <c r="A459">
         <v>4</v>
       </c>
@@ -9859,8 +10330,11 @@
       <c r="H459">
         <v>3</v>
       </c>
-    </row>
-    <row r="460" spans="1:8">
+      <c r="I459" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="460" spans="1:9">
       <c r="A460">
         <v>4</v>
       </c>
@@ -9885,8 +10359,11 @@
       <c r="H460">
         <v>3</v>
       </c>
-    </row>
-    <row r="461" spans="1:8">
+      <c r="I460" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="461" spans="1:9">
       <c r="A461">
         <v>4</v>
       </c>
@@ -9911,8 +10388,11 @@
       <c r="H461">
         <v>6</v>
       </c>
-    </row>
-    <row r="462" spans="1:8">
+      <c r="I461" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="462" spans="1:9">
       <c r="A462">
         <v>4</v>
       </c>
@@ -9937,8 +10417,11 @@
       <c r="H462">
         <v>8</v>
       </c>
-    </row>
-    <row r="463" spans="1:8">
+      <c r="I462" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="463" spans="1:9">
       <c r="A463">
         <v>4</v>
       </c>
@@ -9951,8 +10434,11 @@
       <c r="D463">
         <v>295</v>
       </c>
-    </row>
-    <row r="464" spans="1:8">
+      <c r="I463" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="464" spans="1:9">
       <c r="A464">
         <v>4</v>
       </c>
@@ -9965,8 +10451,11 @@
       <c r="D464">
         <v>302</v>
       </c>
-    </row>
-    <row r="465" spans="1:4">
+      <c r="I464" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="465" spans="1:9">
       <c r="A465">
         <v>4</v>
       </c>
@@ -9979,8 +10468,11 @@
       <c r="D465">
         <v>241</v>
       </c>
-    </row>
-    <row r="466" spans="1:4">
+      <c r="I465" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="466" spans="1:9">
       <c r="A466">
         <v>4</v>
       </c>
@@ -9993,8 +10485,11 @@
       <c r="D466">
         <v>549</v>
       </c>
-    </row>
-    <row r="467" spans="1:4">
+      <c r="I466" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="467" spans="1:9">
       <c r="A467">
         <v>4</v>
       </c>
@@ -10007,8 +10502,11 @@
       <c r="D467">
         <v>24</v>
       </c>
-    </row>
-    <row r="468" spans="1:4">
+      <c r="I467" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="468" spans="1:9">
       <c r="A468">
         <v>4</v>
       </c>
@@ -10021,8 +10519,11 @@
       <c r="D468">
         <v>146</v>
       </c>
-    </row>
-    <row r="469" spans="1:4">
+      <c r="I468" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="469" spans="1:9">
       <c r="A469">
         <v>4</v>
       </c>
@@ -10035,8 +10536,11 @@
       <c r="D469">
         <v>401</v>
       </c>
-    </row>
-    <row r="470" spans="1:4">
+      <c r="I469" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="470" spans="1:9">
       <c r="A470">
         <v>4</v>
       </c>
@@ -10049,8 +10553,11 @@
       <c r="D470">
         <v>151</v>
       </c>
-    </row>
-    <row r="471" spans="1:4">
+      <c r="I470" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="471" spans="1:9">
       <c r="A471">
         <v>4</v>
       </c>
@@ -10063,8 +10570,11 @@
       <c r="D471">
         <v>513</v>
       </c>
-    </row>
-    <row r="472" spans="1:4">
+      <c r="I471" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="472" spans="1:9">
       <c r="A472">
         <v>4</v>
       </c>
@@ -10077,8 +10587,11 @@
       <c r="D472">
         <v>164</v>
       </c>
-    </row>
-    <row r="473" spans="1:4">
+      <c r="I472" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="473" spans="1:9">
       <c r="A473">
         <v>4</v>
       </c>
@@ -10091,8 +10604,11 @@
       <c r="D473">
         <v>6</v>
       </c>
-    </row>
-    <row r="474" spans="1:4">
+      <c r="I473" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="474" spans="1:9">
       <c r="A474">
         <v>4</v>
       </c>
@@ -10105,8 +10621,11 @@
       <c r="D474">
         <v>339</v>
       </c>
-    </row>
-    <row r="475" spans="1:4">
+      <c r="I474" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="475" spans="1:9">
       <c r="A475">
         <v>4</v>
       </c>
@@ -10119,8 +10638,11 @@
       <c r="D475">
         <v>34</v>
       </c>
-    </row>
-    <row r="476" spans="1:4">
+      <c r="I475" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="476" spans="1:9">
       <c r="A476">
         <v>4</v>
       </c>
@@ -10133,8 +10655,11 @@
       <c r="D476">
         <v>499</v>
       </c>
-    </row>
-    <row r="477" spans="1:4">
+      <c r="I476" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="477" spans="1:9">
       <c r="A477">
         <v>4</v>
       </c>
@@ -10147,8 +10672,11 @@
       <c r="D477" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="478" spans="1:4">
+      <c r="I477" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="478" spans="1:9">
       <c r="A478">
         <v>4</v>
       </c>
@@ -10161,8 +10689,11 @@
       <c r="D478">
         <v>516</v>
       </c>
-    </row>
-    <row r="479" spans="1:4">
+      <c r="I478" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="479" spans="1:9">
       <c r="A479">
         <v>4</v>
       </c>
@@ -10175,8 +10706,11 @@
       <c r="D479">
         <v>600</v>
       </c>
-    </row>
-    <row r="480" spans="1:4">
+      <c r="I479" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="480" spans="1:9">
       <c r="A480">
         <v>4</v>
       </c>
@@ -10189,8 +10723,11 @@
       <c r="D480">
         <v>545</v>
       </c>
-    </row>
-    <row r="481" spans="1:8">
+      <c r="I480" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="481" spans="1:9">
       <c r="A481">
         <v>4</v>
       </c>
@@ -10203,8 +10740,11 @@
       <c r="D481" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="482" spans="1:8">
+      <c r="I481" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="482" spans="1:9">
       <c r="A482">
         <v>4</v>
       </c>
@@ -10217,8 +10757,11 @@
       <c r="D482">
         <v>16</v>
       </c>
-    </row>
-    <row r="483" spans="1:8">
+      <c r="I482" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="483" spans="1:9">
       <c r="A483">
         <v>4</v>
       </c>
@@ -10243,8 +10786,11 @@
       <c r="H483">
         <v>3</v>
       </c>
-    </row>
-    <row r="484" spans="1:8">
+      <c r="I483" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="484" spans="1:9">
       <c r="A484">
         <v>4</v>
       </c>
@@ -10269,8 +10815,11 @@
       <c r="H484">
         <v>7</v>
       </c>
-    </row>
-    <row r="485" spans="1:8">
+      <c r="I484" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="485" spans="1:9">
       <c r="A485">
         <v>4</v>
       </c>
@@ -10295,8 +10844,11 @@
       <c r="H485">
         <v>24</v>
       </c>
-    </row>
-    <row r="486" spans="1:8">
+      <c r="I485" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="486" spans="1:9">
       <c r="A486">
         <v>4</v>
       </c>
@@ -10321,8 +10873,11 @@
       <c r="H486">
         <v>9</v>
       </c>
-    </row>
-    <row r="487" spans="1:8">
+      <c r="I486" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="487" spans="1:9">
       <c r="A487">
         <v>4</v>
       </c>
@@ -10335,8 +10890,11 @@
       <c r="D487">
         <v>507</v>
       </c>
-    </row>
-    <row r="488" spans="1:8">
+      <c r="I487" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="488" spans="1:9">
       <c r="A488">
         <v>4</v>
       </c>
@@ -10361,8 +10919,11 @@
       <c r="H488">
         <v>13</v>
       </c>
-    </row>
-    <row r="489" spans="1:8">
+      <c r="I488" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="489" spans="1:9">
       <c r="A489">
         <v>4</v>
       </c>
@@ -10387,8 +10948,11 @@
       <c r="H489">
         <v>8</v>
       </c>
-    </row>
-    <row r="490" spans="1:8">
+      <c r="I489" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="490" spans="1:9">
       <c r="A490">
         <v>4</v>
       </c>
@@ -10401,8 +10965,11 @@
       <c r="D490">
         <v>84</v>
       </c>
-    </row>
-    <row r="491" spans="1:8">
+      <c r="I490" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="491" spans="1:9">
       <c r="A491">
         <v>4</v>
       </c>
@@ -10427,8 +10994,11 @@
       <c r="H491">
         <v>8</v>
       </c>
-    </row>
-    <row r="492" spans="1:8">
+      <c r="I491" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="492" spans="1:9">
       <c r="A492">
         <v>4</v>
       </c>
@@ -10453,8 +11023,11 @@
       <c r="H492">
         <v>14</v>
       </c>
-    </row>
-    <row r="493" spans="1:8">
+      <c r="I492" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="493" spans="1:9">
       <c r="A493">
         <v>4</v>
       </c>
@@ -10467,8 +11040,11 @@
       <c r="D493">
         <v>122</v>
       </c>
-    </row>
-    <row r="494" spans="1:8">
+      <c r="I493" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="494" spans="1:9">
       <c r="A494">
         <v>4</v>
       </c>
@@ -10481,8 +11057,11 @@
       <c r="D494">
         <v>373</v>
       </c>
-    </row>
-    <row r="495" spans="1:8">
+      <c r="I494" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="495" spans="1:9">
       <c r="A495">
         <v>4</v>
       </c>
@@ -10495,8 +11074,11 @@
       <c r="D495">
         <v>399</v>
       </c>
-    </row>
-    <row r="496" spans="1:8">
+      <c r="I495" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="496" spans="1:9">
       <c r="A496">
         <v>4</v>
       </c>
@@ -10521,8 +11103,11 @@
       <c r="H496">
         <v>3</v>
       </c>
-    </row>
-    <row r="497" spans="1:8">
+      <c r="I496" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="497" spans="1:9">
       <c r="A497">
         <v>4</v>
       </c>
@@ -10535,8 +11120,11 @@
       <c r="D497">
         <v>4</v>
       </c>
-    </row>
-    <row r="498" spans="1:8">
+      <c r="I497" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="498" spans="1:9">
       <c r="A498">
         <v>4</v>
       </c>
@@ -10549,8 +11137,11 @@
       <c r="D498">
         <v>40</v>
       </c>
-    </row>
-    <row r="499" spans="1:8">
+      <c r="I498" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="499" spans="1:9">
       <c r="A499">
         <v>4</v>
       </c>
@@ -10563,8 +11154,11 @@
       <c r="D499">
         <v>398</v>
       </c>
-    </row>
-    <row r="500" spans="1:8">
+      <c r="I499" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="500" spans="1:9">
       <c r="A500">
         <v>4</v>
       </c>
@@ -10577,8 +11171,11 @@
       <c r="D500">
         <v>172</v>
       </c>
-    </row>
-    <row r="501" spans="1:8">
+      <c r="I500" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="501" spans="1:9">
       <c r="A501">
         <v>4</v>
       </c>
@@ -10603,8 +11200,11 @@
       <c r="H501">
         <v>5</v>
       </c>
-    </row>
-    <row r="502" spans="1:8">
+      <c r="I501" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="502" spans="1:9">
       <c r="A502">
         <v>4</v>
       </c>
@@ -10617,8 +11217,11 @@
       <c r="D502" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="503" spans="1:8">
+      <c r="I502" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="503" spans="1:9">
       <c r="A503">
         <v>5</v>
       </c>
@@ -10631,8 +11234,11 @@
       <c r="D503" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="504" spans="1:8">
+      <c r="I503" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="504" spans="1:9">
       <c r="A504">
         <v>5</v>
       </c>
@@ -10645,8 +11251,11 @@
       <c r="D504">
         <v>342</v>
       </c>
-    </row>
-    <row r="505" spans="1:8">
+      <c r="I504" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="505" spans="1:9">
       <c r="A505">
         <v>5</v>
       </c>
@@ -10659,8 +11268,11 @@
       <c r="D505">
         <v>561</v>
       </c>
-    </row>
-    <row r="506" spans="1:8">
+      <c r="I505" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="506" spans="1:9">
       <c r="A506">
         <v>5</v>
       </c>
@@ -10673,8 +11285,11 @@
       <c r="D506" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="507" spans="1:8">
+      <c r="I506" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="507" spans="1:9">
       <c r="A507">
         <v>5</v>
       </c>
@@ -10687,8 +11302,11 @@
       <c r="D507">
         <v>336</v>
       </c>
-    </row>
-    <row r="508" spans="1:8">
+      <c r="I507" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="508" spans="1:9">
       <c r="A508">
         <v>5</v>
       </c>
@@ -10713,8 +11331,11 @@
       <c r="H508">
         <v>10</v>
       </c>
-    </row>
-    <row r="509" spans="1:8">
+      <c r="I508" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="509" spans="1:9">
       <c r="A509">
         <v>5</v>
       </c>
@@ -10727,8 +11348,11 @@
       <c r="D509">
         <v>602</v>
       </c>
-    </row>
-    <row r="510" spans="1:8">
+      <c r="I509" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="510" spans="1:9">
       <c r="A510">
         <v>5</v>
       </c>
@@ -10753,8 +11377,11 @@
       <c r="H510">
         <v>17</v>
       </c>
-    </row>
-    <row r="511" spans="1:8">
+      <c r="I510" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="511" spans="1:9">
       <c r="A511">
         <v>5</v>
       </c>
@@ -10767,8 +11394,11 @@
       <c r="D511" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="512" spans="1:8">
+      <c r="I511" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="512" spans="1:9">
       <c r="A512">
         <v>5</v>
       </c>
@@ -10793,8 +11423,11 @@
       <c r="H512">
         <v>7</v>
       </c>
-    </row>
-    <row r="513" spans="1:8">
+      <c r="I512" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="513" spans="1:10">
       <c r="A513">
         <v>5</v>
       </c>
@@ -10819,8 +11452,11 @@
       <c r="H513">
         <v>12</v>
       </c>
-    </row>
-    <row r="514" spans="1:8">
+      <c r="I513" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="514" spans="1:10">
       <c r="A514">
         <v>5</v>
       </c>
@@ -10833,8 +11469,11 @@
       <c r="D514">
         <v>359</v>
       </c>
-    </row>
-    <row r="515" spans="1:8">
+      <c r="I514" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="515" spans="1:10">
       <c r="A515">
         <v>5</v>
       </c>
@@ -10853,8 +11492,11 @@
       <c r="F515">
         <v>211</v>
       </c>
-    </row>
-    <row r="516" spans="1:8">
+      <c r="I515" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="516" spans="1:10">
       <c r="A516">
         <v>5</v>
       </c>
@@ -10867,8 +11509,11 @@
       <c r="D516">
         <v>211</v>
       </c>
-    </row>
-    <row r="517" spans="1:8">
+      <c r="I516" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="517" spans="1:10">
       <c r="A517">
         <v>5</v>
       </c>
@@ -10881,8 +11526,11 @@
       <c r="D517">
         <v>571</v>
       </c>
-    </row>
-    <row r="518" spans="1:8">
+      <c r="I517" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="518" spans="1:10">
       <c r="A518">
         <v>5</v>
       </c>
@@ -10895,8 +11543,11 @@
       <c r="D518">
         <v>377</v>
       </c>
-    </row>
-    <row r="519" spans="1:8">
+      <c r="I518" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="519" spans="1:10">
       <c r="A519">
         <v>5</v>
       </c>
@@ -10909,8 +11560,11 @@
       <c r="D519">
         <v>489</v>
       </c>
-    </row>
-    <row r="520" spans="1:8">
+      <c r="I519" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="520" spans="1:10">
       <c r="A520">
         <v>5</v>
       </c>
@@ -10923,8 +11577,11 @@
       <c r="D520">
         <v>255</v>
       </c>
-    </row>
-    <row r="521" spans="1:8">
+      <c r="I520" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="521" spans="1:10">
       <c r="A521">
         <v>5</v>
       </c>
@@ -10949,8 +11606,11 @@
       <c r="H521">
         <v>1</v>
       </c>
-    </row>
-    <row r="522" spans="1:8">
+      <c r="I521" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="522" spans="1:10">
       <c r="A522">
         <v>5</v>
       </c>
@@ -10963,8 +11623,11 @@
       <c r="D522">
         <v>576</v>
       </c>
-    </row>
-    <row r="523" spans="1:8">
+      <c r="I522" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="523" spans="1:10">
       <c r="A523">
         <v>5</v>
       </c>
@@ -10977,8 +11640,11 @@
       <c r="D523">
         <v>162</v>
       </c>
-    </row>
-    <row r="524" spans="1:8">
+      <c r="I523" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="524" spans="1:10">
       <c r="A524">
         <v>5</v>
       </c>
@@ -10991,8 +11657,11 @@
       <c r="D524">
         <v>490</v>
       </c>
-    </row>
-    <row r="525" spans="1:8">
+      <c r="I524" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="525" spans="1:10">
       <c r="A525">
         <v>5</v>
       </c>
@@ -11017,8 +11686,14 @@
       <c r="H525">
         <v>11</v>
       </c>
-    </row>
-    <row r="526" spans="1:8">
+      <c r="I525" t="s">
+        <v>59</v>
+      </c>
+      <c r="J525" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="526" spans="1:10">
       <c r="A526">
         <v>5</v>
       </c>
@@ -11031,8 +11706,11 @@
       <c r="D526">
         <v>552</v>
       </c>
-    </row>
-    <row r="527" spans="1:8">
+      <c r="I526" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="527" spans="1:10">
       <c r="A527">
         <v>5</v>
       </c>
@@ -11045,8 +11723,11 @@
       <c r="D527">
         <v>32</v>
       </c>
-    </row>
-    <row r="528" spans="1:8">
+      <c r="I527" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="528" spans="1:10">
       <c r="A528">
         <v>5</v>
       </c>
@@ -11059,8 +11740,11 @@
       <c r="D528">
         <v>556</v>
       </c>
-    </row>
-    <row r="529" spans="1:8">
+      <c r="I528" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="529" spans="1:9">
       <c r="A529">
         <v>5</v>
       </c>
@@ -11073,8 +11757,11 @@
       <c r="D529">
         <v>555</v>
       </c>
-    </row>
-    <row r="530" spans="1:8">
+      <c r="I529" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="530" spans="1:9">
       <c r="A530">
         <v>5</v>
       </c>
@@ -11087,8 +11774,11 @@
       <c r="D530">
         <v>303</v>
       </c>
-    </row>
-    <row r="531" spans="1:8">
+      <c r="I530" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="531" spans="1:9">
       <c r="A531">
         <v>5</v>
       </c>
@@ -11101,8 +11791,11 @@
       <c r="D531">
         <v>126</v>
       </c>
-    </row>
-    <row r="532" spans="1:8">
+      <c r="I531" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="532" spans="1:9">
       <c r="A532">
         <v>5</v>
       </c>
@@ -11115,8 +11808,11 @@
       <c r="D532">
         <v>67</v>
       </c>
-    </row>
-    <row r="533" spans="1:8">
+      <c r="I532" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="533" spans="1:9">
       <c r="A533">
         <v>5</v>
       </c>
@@ -11129,8 +11825,11 @@
       <c r="D533">
         <v>345</v>
       </c>
-    </row>
-    <row r="534" spans="1:8">
+      <c r="I533" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="534" spans="1:9">
       <c r="A534">
         <v>5</v>
       </c>
@@ -11143,8 +11842,11 @@
       <c r="D534">
         <v>360</v>
       </c>
-    </row>
-    <row r="535" spans="1:8">
+      <c r="I534" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="535" spans="1:9">
       <c r="A535">
         <v>5</v>
       </c>
@@ -11157,8 +11859,11 @@
       <c r="D535">
         <v>129</v>
       </c>
-    </row>
-    <row r="536" spans="1:8">
+      <c r="I535" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="536" spans="1:9">
       <c r="A536">
         <v>5</v>
       </c>
@@ -11171,8 +11876,11 @@
       <c r="D536">
         <v>69</v>
       </c>
-    </row>
-    <row r="537" spans="1:8">
+      <c r="I536" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="537" spans="1:9">
       <c r="A537">
         <v>5</v>
       </c>
@@ -11185,8 +11893,11 @@
       <c r="D537">
         <v>318</v>
       </c>
-    </row>
-    <row r="538" spans="1:8">
+      <c r="I537" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="538" spans="1:9">
       <c r="A538">
         <v>5</v>
       </c>
@@ -11199,8 +11910,11 @@
       <c r="D538">
         <v>452</v>
       </c>
-    </row>
-    <row r="539" spans="1:8">
+      <c r="I538" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="539" spans="1:9">
       <c r="A539">
         <v>5</v>
       </c>
@@ -11213,8 +11927,11 @@
       <c r="D539">
         <v>485</v>
       </c>
-    </row>
-    <row r="540" spans="1:8">
+      <c r="I539" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="540" spans="1:9">
       <c r="A540">
         <v>5</v>
       </c>
@@ -11227,8 +11944,11 @@
       <c r="D540" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="541" spans="1:8">
+      <c r="I540" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="541" spans="1:9">
       <c r="A541">
         <v>5</v>
       </c>
@@ -11241,8 +11961,11 @@
       <c r="D541" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="542" spans="1:8">
+      <c r="I541" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="542" spans="1:9">
       <c r="A542">
         <v>5</v>
       </c>
@@ -11267,8 +11990,11 @@
       <c r="H542">
         <v>8</v>
       </c>
-    </row>
-    <row r="543" spans="1:8">
+      <c r="I542" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="543" spans="1:9">
       <c r="A543">
         <v>5</v>
       </c>
@@ -11281,8 +12007,11 @@
       <c r="D543" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="544" spans="1:8">
+      <c r="I543" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="544" spans="1:9">
       <c r="A544">
         <v>5</v>
       </c>
@@ -11295,8 +12024,11 @@
       <c r="D544">
         <v>298</v>
       </c>
-    </row>
-    <row r="545" spans="1:8">
+      <c r="I544" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="545" spans="1:9">
       <c r="A545">
         <v>5</v>
       </c>
@@ -11309,8 +12041,11 @@
       <c r="D545">
         <v>48</v>
       </c>
-    </row>
-    <row r="546" spans="1:8">
+      <c r="I545" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="546" spans="1:9">
       <c r="A546">
         <v>5</v>
       </c>
@@ -11335,8 +12070,11 @@
       <c r="H546">
         <v>7</v>
       </c>
-    </row>
-    <row r="547" spans="1:8">
+      <c r="I546" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="547" spans="1:9">
       <c r="A547">
         <v>5</v>
       </c>
@@ -11361,8 +12099,11 @@
       <c r="H547">
         <v>5</v>
       </c>
-    </row>
-    <row r="548" spans="1:8">
+      <c r="I547" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="548" spans="1:9">
       <c r="A548">
         <v>5</v>
       </c>
@@ -11387,8 +12128,11 @@
       <c r="H548">
         <v>3</v>
       </c>
-    </row>
-    <row r="549" spans="1:8">
+      <c r="I548" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="549" spans="1:9">
       <c r="A549">
         <v>5</v>
       </c>
@@ -11401,8 +12145,11 @@
       <c r="D549">
         <v>33</v>
       </c>
-    </row>
-    <row r="550" spans="1:8">
+      <c r="I549" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="550" spans="1:9">
       <c r="A550">
         <v>5</v>
       </c>
@@ -11415,8 +12162,11 @@
       <c r="D550">
         <v>26</v>
       </c>
-    </row>
-    <row r="551" spans="1:8">
+      <c r="I550" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="551" spans="1:9">
       <c r="A551">
         <v>5</v>
       </c>
@@ -11429,8 +12179,11 @@
       <c r="D551">
         <v>413</v>
       </c>
-    </row>
-    <row r="552" spans="1:8">
+      <c r="I551" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="552" spans="1:9">
       <c r="A552">
         <v>5</v>
       </c>
@@ -11443,8 +12196,11 @@
       <c r="D552">
         <v>464</v>
       </c>
-    </row>
-    <row r="553" spans="1:8">
+      <c r="I552" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="553" spans="1:9">
       <c r="A553">
         <v>5</v>
       </c>
@@ -11469,8 +12225,11 @@
       <c r="H553">
         <v>8</v>
       </c>
-    </row>
-    <row r="554" spans="1:8">
+      <c r="I553" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="554" spans="1:9">
       <c r="A554">
         <v>5</v>
       </c>
@@ -11483,8 +12242,11 @@
       <c r="D554">
         <v>568</v>
       </c>
-    </row>
-    <row r="555" spans="1:8">
+      <c r="I554" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="555" spans="1:9">
       <c r="A555">
         <v>5</v>
       </c>
@@ -11497,8 +12259,11 @@
       <c r="D555">
         <v>348</v>
       </c>
-    </row>
-    <row r="556" spans="1:8">
+      <c r="I555" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="556" spans="1:9">
       <c r="A556">
         <v>5</v>
       </c>
@@ -11511,8 +12276,11 @@
       <c r="D556">
         <v>558</v>
       </c>
-    </row>
-    <row r="557" spans="1:8">
+      <c r="I556" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="557" spans="1:9">
       <c r="A557">
         <v>5</v>
       </c>
@@ -11525,8 +12293,11 @@
       <c r="D557">
         <v>563</v>
       </c>
-    </row>
-    <row r="558" spans="1:8">
+      <c r="I557" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="558" spans="1:9">
       <c r="A558">
         <v>5</v>
       </c>
@@ -11538,6 +12309,9 @@
       </c>
       <c r="D558">
         <v>363</v>
+      </c>
+      <c r="I558" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>